<commit_message>
Update Test on Basler Sensor
</commit_message>
<xml_diff>
--- a/tests/test.xlsx
+++ b/tests/test.xlsx
@@ -8,40 +8,103 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="J:\_tools\git_repo\LEnsE\ressources\lensecam\tests\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A18A5ED7-AAB2-4B56-A7D5-5927F2D36531}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{13303D26-4EF3-4E29-8BE3-D6472089FE5E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="24240" windowHeight="13140" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="24240" windowHeight="13140" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Feuil1" sheetId="1" r:id="rId1"/>
+    <sheet name="Flux" sheetId="1" r:id="rId1"/>
+    <sheet name="Obscurité" sheetId="2" r:id="rId2"/>
+    <sheet name="Couleur" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3" uniqueCount="3">
-  <si>
-    <t>T</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="17">
   <si>
     <t>Mean 1</t>
   </si>
   <si>
     <t>Mean 2</t>
   </si>
+  <si>
+    <t>T (us)</t>
+  </si>
+  <si>
+    <t>T (ms)</t>
+  </si>
+  <si>
+    <t>Std1</t>
+  </si>
+  <si>
+    <t>Std2</t>
+  </si>
+  <si>
+    <t>Test with Pylon Viewer 8</t>
+  </si>
+  <si>
+    <t>Mean1-m0</t>
+  </si>
+  <si>
+    <t>BL = 4</t>
+  </si>
+  <si>
+    <t>Std1^2-Std0^2</t>
+  </si>
+  <si>
+    <t>sqrt( )</t>
+  </si>
+  <si>
+    <t>Mean1 - m0</t>
+  </si>
+  <si>
+    <t>lambda</t>
+  </si>
+  <si>
+    <t>ROI : 200 x 200</t>
+  </si>
+  <si>
+    <t>T = 50 ms</t>
+  </si>
+  <si>
+    <t>Lampe</t>
+  </si>
+  <si>
+    <t>I = 2,2A / V = 23,3V</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -69,8 +132,19 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -173,7 +247,7 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>Feuil1!$B$1</c:f>
+              <c:f>Flux!$B$3</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -221,7 +295,7 @@
           </c:trendline>
           <c:xVal>
             <c:numRef>
-              <c:f>Feuil1!$A$2:$A$7</c:f>
+              <c:f>Flux!$A$4:$A$9</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="6"/>
@@ -248,7 +322,7 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Feuil1!$B$2:$B$7</c:f>
+              <c:f>Flux!$B$4:$B$9</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="6"/>
@@ -285,7 +359,7 @@
           <c:order val="1"/>
           <c:tx>
             <c:strRef>
-              <c:f>Feuil1!$C$1</c:f>
+              <c:f>Flux!$D$3</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -333,7 +407,7 @@
           </c:trendline>
           <c:xVal>
             <c:numRef>
-              <c:f>Feuil1!$A$2:$A$12</c:f>
+              <c:f>Flux!$A$4:$A$14</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="11"/>
@@ -375,7 +449,7 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Feuil1!$C$2:$C$12</c:f>
+              <c:f>Flux!$D$4:$D$14</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="11"/>
@@ -754,7 +828,1556 @@
 </c:chartSpace>
 </file>
 
+<file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="fr-FR"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US"/>
+              <a:t>Intensité</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="en-US" baseline="0"/>
+              <a:t> moyenne - Obscurité</a:t>
+            </a:r>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="fr-FR"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:scatterChart>
+        <c:scatterStyle val="lineMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Obscurité!$B$3</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Mean 1</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:noFill/>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Obscurité!$A$4:$A$18</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="15"/>
+                <c:pt idx="0">
+                  <c:v>20</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1000</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>5000</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>10000</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>20000</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>50000</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>70000</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>100000</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>200000</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>300000</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>400000</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>500000</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>700000</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>800000</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>1000000</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Obscurité!$B$4:$B$18</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="15"/>
+                <c:pt idx="0">
+                  <c:v>2.96</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2.96</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>2.96</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>2.97</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>3.08</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>3.13</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>3.22</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>3.51</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>3.8</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>4.0999999999999996</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>2.5</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>1.31</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>1.61</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>1.4</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-E37A-4EF7-B730-4AB91D81177F}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="505856816"/>
+        <c:axId val="505856096"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="505856816"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+          <c:max val="1000000"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="fr-FR"/>
+                  <a:t>Temps Intégration (us)</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="fr-FR"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="fr-FR"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="505856096"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="505856096"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>ADU</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="fr-FR"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="fr-FR"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="505856816"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="fr-FR"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart3.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="fr-FR"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="fr-FR"/>
+              <a:t>Bruit - Obscurité</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="fr-FR"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:scatterChart>
+        <c:scatterStyle val="lineMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Obscurité!$F$3</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>sqrt( )</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:noFill/>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Obscurité!$A$4:$A$18</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="15"/>
+                <c:pt idx="0">
+                  <c:v>20</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1000</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>5000</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>10000</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>20000</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>50000</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>70000</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>100000</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>200000</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>300000</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>400000</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>500000</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>700000</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>800000</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>1000000</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Obscurité!$F$4:$F$18</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="15"/>
+                <c:pt idx="1">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.10344080432788594</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.11810588469674146</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.18083141320025126</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.23558437978779481</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0.28124722220850457</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0.48733971724044811</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>0.67727394752788173</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>0.87149297185921126</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>1.076615065842941</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>1.403246236410417</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>1.6152708751166165</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>2.0320187007013493</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-0811-4535-9600-0E08B8611831}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="627724984"/>
+        <c:axId val="627725344"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="627724984"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+          <c:max val="1000000"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="fr-FR"/>
+                  <a:t>Temps Intégration (us)</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="fr-FR"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="fr-FR"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="627725344"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="627725344"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="fr-FR"/>
+                  <a:t>ADU</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="fr-FR"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="fr-FR"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="627724984"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="fr-FR"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart4.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="fr-FR"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US"/>
+              <a:t>Réponse spectrale</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="fr-FR"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:scatterChart>
+        <c:scatterStyle val="lineMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Couleur!$C$3</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Mean1 - m0</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:noFill/>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Couleur!$A$4:$A$12</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="9"/>
+                <c:pt idx="0">
+                  <c:v>400</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>450</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>500</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>550</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>600</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>630</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>650</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>700</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>750</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Couleur!$C$4:$C$12</c:f>
+              <c:numCache>
+                <c:formatCode>0</c:formatCode>
+                <c:ptCount val="9"/>
+                <c:pt idx="0">
+                  <c:v>54.92</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>151.91999999999999</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1385.92</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>2346.92</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>2760.92</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>2010.92</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>411.92</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>6.92</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>4.92</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-C897-4A92-871F-ECDB1F63213D}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="505857176"/>
+        <c:axId val="440030024"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="505857176"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+          <c:max val="750"/>
+          <c:min val="400"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="fr-FR"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="440030024"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="440030024"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="0" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="fr-FR"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="505857176"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="fr-FR"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
 <file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/colors2.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/colors3.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/colors4.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
   <a:schemeClr val="accent1"/>
   <a:schemeClr val="accent2"/>
@@ -1310,20 +2933,1568 @@
 </cs:chartStyle>
 </file>
 
+<file path=xl/charts/style2.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style3.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style4.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>3</xdr:col>
-      <xdr:colOff>485775</xdr:colOff>
-      <xdr:row>2</xdr:row>
-      <xdr:rowOff>138112</xdr:rowOff>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>266700</xdr:colOff>
+      <xdr:row>4</xdr:row>
+      <xdr:rowOff>23812</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>13</xdr:col>
-      <xdr:colOff>28575</xdr:colOff>
-      <xdr:row>22</xdr:row>
-      <xdr:rowOff>133350</xdr:rowOff>
+      <xdr:col>15</xdr:col>
+      <xdr:colOff>419100</xdr:colOff>
+      <xdr:row>24</xdr:row>
+      <xdr:rowOff>19050</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -1331,6 +4502,124 @@
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
               <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{A2314FA5-9340-443F-18ED-98FCA15242FB}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>495300</xdr:colOff>
+      <xdr:row>3</xdr:row>
+      <xdr:rowOff>4762</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>495300</xdr:colOff>
+      <xdr:row>17</xdr:row>
+      <xdr:rowOff>80962</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Graphique 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{B2468944-59B8-1CBE-909A-06FADC50DECC}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>495300</xdr:colOff>
+      <xdr:row>18</xdr:row>
+      <xdr:rowOff>33337</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>495300</xdr:colOff>
+      <xdr:row>32</xdr:row>
+      <xdr:rowOff>109537</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="4" name="Graphique 3">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{1826D4B4-38F8-61B2-7B1B-F93262097B43}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing3.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>414336</xdr:colOff>
+      <xdr:row>2</xdr:row>
+      <xdr:rowOff>138111</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>723899</xdr:colOff>
+      <xdr:row>21</xdr:row>
+      <xdr:rowOff>85724</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Graphique 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{54B5E86A-0F07-E82A-0E31-F677145262F5}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1614,129 +4903,687 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:C12"/>
+  <dimension ref="A1:E14"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C17" sqref="C17"/>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:E14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>3</v>
+      </c>
+      <c r="B3" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
+      <c r="C3" t="s">
+        <v>4</v>
+      </c>
+      <c r="D3" t="s">
         <v>1</v>
       </c>
-      <c r="C1" t="s">
+      <c r="E3" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A4">
+        <v>200</v>
+      </c>
+      <c r="B4">
+        <v>670</v>
+      </c>
+      <c r="D4">
+        <v>350</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A5">
+        <v>500</v>
+      </c>
+      <c r="B5">
+        <v>1640</v>
+      </c>
+      <c r="D5">
+        <v>820</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A6">
+        <v>800</v>
+      </c>
+      <c r="B6">
+        <v>2600</v>
+      </c>
+      <c r="D6">
+        <v>1300</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A7">
+        <v>1100</v>
+      </c>
+      <c r="B7">
+        <v>3330</v>
+      </c>
+      <c r="D7">
+        <v>1770</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A8">
+        <v>1400</v>
+      </c>
+      <c r="B8">
+        <v>3580</v>
+      </c>
+      <c r="D8">
+        <v>2250</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A9">
+        <v>1600</v>
+      </c>
+      <c r="B9">
+        <v>3750</v>
+      </c>
+      <c r="D9">
+        <v>2600</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A10">
+        <v>2000</v>
+      </c>
+      <c r="D10">
+        <v>3170</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A11">
+        <v>2200</v>
+      </c>
+      <c r="D11">
+        <v>3310</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A12">
+        <v>2500</v>
+      </c>
+      <c r="D12">
+        <v>3435</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A13">
+        <v>3000</v>
+      </c>
+      <c r="D13">
+        <v>3640</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A14">
+        <v>4000</v>
+      </c>
+      <c r="D14">
+        <v>3950</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CAEAFC4E-FCF5-436F-9346-481F878ADA69}">
+  <dimension ref="A1:F18"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E8" sqref="E8"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="6" width="11.42578125" style="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A1" s="2" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="C2" s="3" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A3" s="3" t="s">
         <v>2</v>
       </c>
+      <c r="B3" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="E3" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="F3" s="1" t="s">
+        <v>10</v>
+      </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A2">
-        <v>200</v>
-      </c>
-      <c r="B2">
-        <v>670</v>
-      </c>
-      <c r="C2">
-        <v>350</v>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A4" s="3">
+        <v>20</v>
+      </c>
+      <c r="B4" s="1">
+        <v>2.96</v>
+      </c>
+      <c r="D4" s="1">
+        <v>0.53</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A3">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A5" s="3">
+        <v>1000</v>
+      </c>
+      <c r="B5" s="1">
+        <v>2.96</v>
+      </c>
+      <c r="C5" s="1">
+        <f>B5-$B$4</f>
+        <v>0</v>
+      </c>
+      <c r="D5" s="1">
+        <v>0.53</v>
+      </c>
+      <c r="E5" s="1">
+        <f>D5*D5-$D$4*$D$4</f>
+        <v>0</v>
+      </c>
+      <c r="F5" s="1">
+        <f>SQRT(E5)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A6" s="3">
+        <v>5000</v>
+      </c>
+      <c r="B6" s="1">
+        <v>2.96</v>
+      </c>
+      <c r="C6" s="1">
+        <f t="shared" ref="C6:C18" si="0">B6-$B$4</f>
+        <v>0</v>
+      </c>
+      <c r="D6" s="1">
+        <v>0.53</v>
+      </c>
+      <c r="E6" s="1">
+        <f>D6*D6-$D$4*$D$4</f>
+        <v>0</v>
+      </c>
+      <c r="F6" s="1">
+        <f t="shared" ref="F6:F18" si="1">SQRT(E6)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A7" s="3">
+        <v>10000</v>
+      </c>
+      <c r="B7" s="1">
+        <v>2.97</v>
+      </c>
+      <c r="C7" s="1">
+        <f t="shared" si="0"/>
+        <v>1.0000000000000231E-2</v>
+      </c>
+      <c r="D7" s="1">
+        <v>0.54</v>
+      </c>
+      <c r="E7" s="1">
+        <f>D7*D7-$D$4*$D$4</f>
+        <v>1.0699999999999987E-2</v>
+      </c>
+      <c r="F7" s="1">
+        <f t="shared" si="1"/>
+        <v>0.10344080432788594</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A8" s="3">
+        <v>20000</v>
+      </c>
+      <c r="B8" s="1">
+        <v>3</v>
+      </c>
+      <c r="C8" s="1">
+        <f t="shared" si="0"/>
+        <v>4.0000000000000036E-2</v>
+      </c>
+      <c r="D8" s="1">
+        <v>0.54300000000000004</v>
+      </c>
+      <c r="E8" s="1">
+        <f>D8*D8-$D$4*$D$4</f>
+        <v>1.3948999999999989E-2</v>
+      </c>
+      <c r="F8" s="1">
+        <f t="shared" si="1"/>
+        <v>0.11810588469674146</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A9" s="3">
+        <v>50000</v>
+      </c>
+      <c r="B9" s="1">
+        <v>3.08</v>
+      </c>
+      <c r="C9" s="1">
+        <f t="shared" si="0"/>
+        <v>0.12000000000000011</v>
+      </c>
+      <c r="D9" s="1">
+        <v>0.56000000000000005</v>
+      </c>
+      <c r="E9" s="1">
+        <f>D9*D9-$D$4*$D$4</f>
+        <v>3.2700000000000007E-2</v>
+      </c>
+      <c r="F9" s="1">
+        <f t="shared" si="1"/>
+        <v>0.18083141320025126</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A10" s="3">
+        <v>70000</v>
+      </c>
+      <c r="B10" s="1">
+        <v>3.13</v>
+      </c>
+      <c r="C10" s="1">
+        <f t="shared" si="0"/>
+        <v>0.16999999999999993</v>
+      </c>
+      <c r="D10" s="1">
+        <v>0.57999999999999996</v>
+      </c>
+      <c r="E10" s="1">
+        <f>D10*D10-$D$4*$D$4</f>
+        <v>5.5499999999999938E-2</v>
+      </c>
+      <c r="F10" s="1">
+        <f t="shared" si="1"/>
+        <v>0.23558437978779481</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A11" s="3">
+        <v>100000</v>
+      </c>
+      <c r="B11" s="1">
+        <v>3.22</v>
+      </c>
+      <c r="C11" s="1">
+        <f t="shared" si="0"/>
+        <v>0.26000000000000023</v>
+      </c>
+      <c r="D11" s="1">
+        <v>0.6</v>
+      </c>
+      <c r="E11" s="1">
+        <f>D11*D11-$D$4*$D$4</f>
+        <v>7.9099999999999948E-2</v>
+      </c>
+      <c r="F11" s="1">
+        <f t="shared" si="1"/>
+        <v>0.28124722220850457</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A12" s="3">
+        <v>200000</v>
+      </c>
+      <c r="B12" s="1">
+        <v>3.51</v>
+      </c>
+      <c r="C12" s="1">
+        <f t="shared" si="0"/>
+        <v>0.54999999999999982</v>
+      </c>
+      <c r="D12" s="1">
+        <v>0.72</v>
+      </c>
+      <c r="E12" s="1">
+        <f>D12*D12-$D$4*$D$4</f>
+        <v>0.23749999999999993</v>
+      </c>
+      <c r="F12" s="1">
+        <f t="shared" si="1"/>
+        <v>0.48733971724044811</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A13" s="3">
+        <v>300000</v>
+      </c>
+      <c r="B13" s="1">
+        <v>3.8</v>
+      </c>
+      <c r="C13" s="1">
+        <f t="shared" si="0"/>
+        <v>0.83999999999999986</v>
+      </c>
+      <c r="D13" s="1">
+        <v>0.86</v>
+      </c>
+      <c r="E13" s="1">
+        <f>D13*D13-$D$4*$D$4</f>
+        <v>0.45869999999999989</v>
+      </c>
+      <c r="F13" s="1">
+        <f t="shared" si="1"/>
+        <v>0.67727394752788173</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A14" s="3">
+        <v>400000</v>
+      </c>
+      <c r="B14" s="1">
+        <v>4.0999999999999996</v>
+      </c>
+      <c r="C14" s="1">
+        <f t="shared" si="0"/>
+        <v>1.1399999999999997</v>
+      </c>
+      <c r="D14" s="1">
+        <v>1.02</v>
+      </c>
+      <c r="E14" s="1">
+        <f>D14*D14-$D$4*$D$4</f>
+        <v>0.75949999999999995</v>
+      </c>
+      <c r="F14" s="1">
+        <f t="shared" si="1"/>
+        <v>0.87149297185921126</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A15" s="3">
+        <v>500000</v>
+      </c>
+      <c r="B15" s="1">
+        <v>2.5</v>
+      </c>
+      <c r="C15" s="1">
+        <f t="shared" si="0"/>
+        <v>-0.45999999999999996</v>
+      </c>
+      <c r="D15" s="1">
+        <v>1.2</v>
+      </c>
+      <c r="E15" s="1">
+        <f>D15*D15-$D$4*$D$4</f>
+        <v>1.1591</v>
+      </c>
+      <c r="F15" s="1">
+        <f t="shared" si="1"/>
+        <v>1.076615065842941</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A16" s="3">
+        <v>700000</v>
+      </c>
+      <c r="B16" s="1">
+        <v>1.31</v>
+      </c>
+      <c r="C16" s="1">
+        <f t="shared" si="0"/>
+        <v>-1.65</v>
+      </c>
+      <c r="D16" s="1">
+        <v>1.5</v>
+      </c>
+      <c r="E16" s="1">
+        <f>D16*D16-$D$4*$D$4</f>
+        <v>1.9691000000000001</v>
+      </c>
+      <c r="F16" s="1">
+        <f t="shared" si="1"/>
+        <v>1.403246236410417</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A17" s="3">
+        <v>800000</v>
+      </c>
+      <c r="B17" s="1">
+        <v>1.61</v>
+      </c>
+      <c r="C17" s="1">
+        <f t="shared" si="0"/>
+        <v>-1.3499999999999999</v>
+      </c>
+      <c r="D17" s="1">
+        <v>1.7</v>
+      </c>
+      <c r="E17" s="1">
+        <f>D17*D17-$D$4*$D$4</f>
+        <v>2.6090999999999998</v>
+      </c>
+      <c r="F17" s="1">
+        <f t="shared" si="1"/>
+        <v>1.6152708751166165</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A18" s="3">
+        <v>1000000</v>
+      </c>
+      <c r="B18" s="1">
+        <v>1.4</v>
+      </c>
+      <c r="C18" s="1">
+        <f t="shared" si="0"/>
+        <v>-1.56</v>
+      </c>
+      <c r="D18" s="1">
+        <v>2.1</v>
+      </c>
+      <c r="E18" s="1">
+        <f>D18*D18-$D$4*$D$4</f>
+        <v>4.1291000000000002</v>
+      </c>
+      <c r="F18" s="1">
+        <f t="shared" si="1"/>
+        <v>2.0320187007013493</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{80E75F14-456C-462A-8A26-8D8F6CA358BB}">
+  <dimension ref="A1:I12"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E3" sqref="E3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>6</v>
+      </c>
+      <c r="E1" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="C2" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="D2" t="s">
+        <v>14</v>
+      </c>
+      <c r="E2">
+        <v>3.08</v>
+      </c>
+      <c r="H2" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="I2" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A3" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="D3" s="1"/>
+      <c r="E3" s="1"/>
+      <c r="F3" s="1"/>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A4">
+        <v>400</v>
+      </c>
+      <c r="B4">
+        <v>58</v>
+      </c>
+      <c r="C4" s="5">
+        <f>B4-$E$2</f>
+        <v>54.92</v>
+      </c>
+      <c r="E4" s="1"/>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A5">
+        <v>450</v>
+      </c>
+      <c r="B5">
+        <v>155</v>
+      </c>
+      <c r="C5" s="5">
+        <f t="shared" ref="C5:C12" si="0">B5-$E$2</f>
+        <v>151.91999999999999</v>
+      </c>
+      <c r="E5" s="1"/>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A6">
         <v>500</v>
       </c>
-      <c r="B3">
-        <v>1640</v>
-      </c>
-      <c r="C3">
-        <v>820</v>
+      <c r="B6">
+        <v>1389</v>
+      </c>
+      <c r="C6" s="5">
+        <f t="shared" si="0"/>
+        <v>1385.92</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A4">
-        <v>800</v>
-      </c>
-      <c r="B4">
-        <v>2600</v>
-      </c>
-      <c r="C4">
-        <v>1300</v>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A7">
+        <v>550</v>
+      </c>
+      <c r="B7">
+        <v>2350</v>
+      </c>
+      <c r="C7" s="5">
+        <f t="shared" si="0"/>
+        <v>2346.92</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A5">
-        <v>1100</v>
-      </c>
-      <c r="B5">
-        <v>3330</v>
-      </c>
-      <c r="C5">
-        <v>1770</v>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A8">
+        <v>600</v>
+      </c>
+      <c r="B8">
+        <v>2764</v>
+      </c>
+      <c r="C8" s="5">
+        <f t="shared" si="0"/>
+        <v>2760.92</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A6">
-        <v>1400</v>
-      </c>
-      <c r="B6">
-        <v>3580</v>
-      </c>
-      <c r="C6">
-        <v>2250</v>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A9">
+        <v>630</v>
+      </c>
+      <c r="B9">
+        <v>2014</v>
+      </c>
+      <c r="C9" s="5">
+        <f t="shared" si="0"/>
+        <v>2010.92</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A7">
-        <v>1600</v>
-      </c>
-      <c r="B7">
-        <v>3750</v>
-      </c>
-      <c r="C7">
-        <v>2600</v>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A10">
+        <v>650</v>
+      </c>
+      <c r="B10">
+        <v>415</v>
+      </c>
+      <c r="C10" s="5">
+        <f t="shared" si="0"/>
+        <v>411.92</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A8">
-        <v>2000</v>
-      </c>
-      <c r="C8">
-        <v>3170</v>
+    <row r="11" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A11">
+        <v>700</v>
+      </c>
+      <c r="B11">
+        <v>10</v>
+      </c>
+      <c r="C11" s="5">
+        <f t="shared" si="0"/>
+        <v>6.92</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A9">
-        <v>2200</v>
-      </c>
-      <c r="C9">
-        <v>3310</v>
-      </c>
-    </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A10">
-        <v>2500</v>
-      </c>
-      <c r="C10">
-        <v>3435</v>
-      </c>
-    </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A11">
-        <v>3000</v>
-      </c>
-      <c r="C11">
-        <v>3640</v>
-      </c>
-    </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12">
-        <v>4000</v>
-      </c>
-      <c r="C12">
-        <v>3950</v>
+        <v>750</v>
+      </c>
+      <c r="B12">
+        <v>8</v>
+      </c>
+      <c r="C12" s="5">
+        <f t="shared" si="0"/>
+        <v>4.92</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
New Test on Basler
</commit_message>
<xml_diff>
--- a/tests/test.xlsx
+++ b/tests/test.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="29127"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="29231"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="J:\_tools\git_repo\LEnsE\ressources\lensecam\tests\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{264621C9-CE01-4CAE-9DC8-76C8A874C4D4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6E2FD1C0-A1AD-4634-BE01-8D9810758074}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="24240" windowHeight="13140" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="9135" yWindow="165" windowWidth="14565" windowHeight="12240" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Flux" sheetId="1" r:id="rId1"/>
@@ -2437,7 +2437,7 @@
         <c:axId val="505857176"/>
         <c:scaling>
           <c:orientation val="minMax"/>
-          <c:max val="750"/>
+          <c:max val="900"/>
           <c:min val="400"/>
         </c:scaling>
         <c:delete val="0"/>
@@ -5550,15 +5550,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>3</xdr:col>
-      <xdr:colOff>414336</xdr:colOff>
+      <xdr:colOff>728661</xdr:colOff>
       <xdr:row>2</xdr:row>
-      <xdr:rowOff>138111</xdr:rowOff>
+      <xdr:rowOff>109536</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>10</xdr:col>
-      <xdr:colOff>723899</xdr:colOff>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>276224</xdr:colOff>
       <xdr:row>21</xdr:row>
-      <xdr:rowOff>85724</xdr:rowOff>
+      <xdr:rowOff>57149</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -5995,7 +5995,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CAEAFC4E-FCF5-436F-9346-481F878ADA69}">
   <dimension ref="A1:F18"/>
   <sheetViews>
-    <sheetView topLeftCell="A5" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="E8" sqref="E8"/>
     </sheetView>
   </sheetViews>
@@ -6377,8 +6377,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{80E75F14-456C-462A-8A26-8D8F6CA358BB}">
   <dimension ref="A1:I12"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E3" sqref="E3"/>
+    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="B23" sqref="B23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>